<commit_message>
modificaciones de las ramas y documentacion
</commit_message>
<xml_diff>
--- a/ProyectoBDEmpresaTransporte/BDSql/Diccionario de datos.xlsx
+++ b/ProyectoBDEmpresaTransporte/BDSql/Diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cba425722e35f70/Documentos/GitHub/proyectoIngDatos/ProyectoBDEmpresaTransporte/BDSql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{180982F0-453E-420C-85DF-C2ACD85E2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{180982F0-453E-420C-85DF-C2ACD85E2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B3BDC01-B425-436E-9248-749DC9CDF3B6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2D468CDA-0F64-4069-ABBB-259ABB56850C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="137">
   <si>
     <t>Proveedor</t>
   </si>
@@ -419,6 +419,36 @@
   </si>
   <si>
     <t>Punto de llegada del recorrido del transporte</t>
+  </si>
+  <si>
+    <t>nombreCliente</t>
+  </si>
+  <si>
+    <t>VARHCHAR</t>
+  </si>
+  <si>
+    <t>Primer nombre y primer apellido del cliente</t>
+  </si>
+  <si>
+    <t>tipoGasto</t>
+  </si>
+  <si>
+    <t>Tipo de gasto 1 = Reparaciones, 2 = Multa , 3 = Otros gastos</t>
+  </si>
+  <si>
+    <t>NOT null</t>
+  </si>
+  <si>
+    <t>estadoConductor</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>El  estado del conductor puede ser activo o inactivo</t>
+  </si>
+  <si>
+    <t>Nombre del gasto</t>
   </si>
 </sst>
 </file>
@@ -739,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -797,6 +827,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -809,9 +848,24 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,21 +876,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -845,17 +884,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,28 +1312,28 @@
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1385,34 +1433,34 @@
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="29">
         <v>45423</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1539,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A3BA74-A845-42A0-AB40-66C7849756A8}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="E21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,12 +1608,12 @@
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
       <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1578,18 +1626,18 @@
       <c r="M1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="33">
         <v>45755</v>
       </c>
       <c r="C2" s="34"/>
@@ -1598,7 +1646,7 @@
       <c r="G2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="33">
         <v>45755</v>
       </c>
       <c r="I2" s="34"/>
@@ -1607,7 +1655,7 @@
       <c r="M2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="27">
+      <c r="N2" s="33">
         <v>45755</v>
       </c>
       <c r="O2" s="34"/>
@@ -1618,30 +1666,30 @@
       <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
       <c r="G3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
       <c r="M3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="30"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -1755,7 +1803,7 @@
         <v>11.8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>68</v>
@@ -1800,7 +1848,7 @@
         <v>11.8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>69</v>
@@ -1839,7 +1887,7 @@
         <v>62</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
@@ -1865,11 +1913,26 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="12">
+        <v>20</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>129</v>
+      </c>
       <c r="G9" s="17" t="s">
         <v>63</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="12" t="s">
@@ -1897,7 +1960,7 @@
         <v>64</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
@@ -1925,7 +1988,7 @@
         <v>65</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="12" t="s">
@@ -1969,27 +2032,27 @@
       <c r="A13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
       <c r="G13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="33"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="33">
         <v>45755</v>
       </c>
       <c r="C14" s="34"/>
@@ -1998,7 +2061,7 @@
       <c r="G14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="33">
         <v>45755</v>
       </c>
       <c r="I14" s="34"/>
@@ -2009,30 +2072,30 @@
       <c r="A15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
       <c r="G15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
       <c r="M15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="33"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="32"/>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -2068,7 +2131,7 @@
       <c r="M16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="27">
+      <c r="N16" s="33">
         <v>45755</v>
       </c>
       <c r="O16" s="34"/>
@@ -2105,12 +2168,12 @@
       <c r="M17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="30"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="38"/>
     </row>
     <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
@@ -2174,7 +2237,7 @@
         <v>54</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>20</v>
@@ -2186,7 +2249,7 @@
         <v>39</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="M19" s="16" t="s">
         <v>117</v>
@@ -2202,7 +2265,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>46</v>
       </c>
@@ -2216,11 +2279,21 @@
       <c r="E20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
+      <c r="G20" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2">
+        <v>20</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="M20" s="16" t="s">
         <v>119</v>
       </c>
@@ -2237,7 +2310,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>47</v>
       </c>
@@ -2251,15 +2324,6 @@
       <c r="E21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33"/>
       <c r="M21" s="16" t="s">
         <v>120</v>
       </c>
@@ -2290,15 +2354,15 @@
       <c r="E22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="27">
-        <v>45755</v>
-      </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="35"/>
+      <c r="G22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="32"/>
       <c r="M22" s="16" t="s">
         <v>121</v>
       </c>
@@ -2315,7 +2379,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>49</v>
       </c>
@@ -2331,15 +2395,15 @@
       <c r="E23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="30"/>
+      <c r="G23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="46">
+        <v>45755</v>
+      </c>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="48"/>
       <c r="M23" s="16" t="s">
         <v>122</v>
       </c>
@@ -2354,78 +2418,86 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="G24" s="18" t="s">
+    <row r="24" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="45"/>
+    </row>
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H25" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="J25" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="K25" s="21" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="G25" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="G26" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" s="2">
-        <v>11.3</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="G27" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="2">
+        <v>11.3</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="G28" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="2">
-        <v>20</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="G28" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="H28" s="8" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="I28" s="2">
         <v>20</v>
@@ -2434,22 +2506,29 @@
         <v>89</v>
       </c>
       <c r="K28" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="2">
+        <v>20</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="9" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H24:K24"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="H1:K1"/>
@@ -2459,6 +2538,16 @@
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion diccionario y documento acorde  correcion de  la docente
</commit_message>
<xml_diff>
--- a/ProyectoBDEmpresaTransporte/BDSql/Diccionario de datos.xlsx
+++ b/ProyectoBDEmpresaTransporte/BDSql/Diccionario de datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cba425722e35f70/Documentos/GitHub/proyectoIngDatos/ProyectoBDEmpresaTransporte/BDSql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crai-portatil.UROSARIO\Documents\GitHub\proyectoIngDatos\ProyectoBDEmpresaTransporte\BDSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{180982F0-453E-420C-85DF-C2ACD85E2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B3BDC01-B425-436E-9248-749DC9CDF3B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92B31DD-B748-47A3-A376-71C673280420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{2D468CDA-0F64-4069-ABBB-259ABB56850C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2D468CDA-0F64-4069-ABBB-259ABB56850C}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionarios datos" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="140">
   <si>
     <t>Proveedor</t>
   </si>
@@ -449,13 +447,22 @@
   </si>
   <si>
     <t>Nombre del gasto</t>
+  </si>
+  <si>
+    <t>FechaViaje</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>indica la fecha en la que se realizo el viaje, es no nulo por la importancia de esta a la hora de tomar decisiones administrativas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,6 +843,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -848,6 +858,51 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -856,54 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1300,42 +1307,42 @@
       <selection sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="3" width="10.25" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="39.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="30">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1352,117 +1359,117 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="30">
         <v>45423</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="28.5">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1545,7 +1552,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1558,7 +1565,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1589,22 +1596,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A3BA74-A845-42A0-AB40-66C7849756A8}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:K23"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="1" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="30.375" customWidth="1"/>
+    <col min="7" max="7" width="18.125" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
     <col min="17" max="17" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1617,81 +1624,81 @@
       <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
       <c r="M1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="37">
         <v>45755</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
       <c r="G2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="33">
+      <c r="H2" s="37">
         <v>45755</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="35"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
       <c r="M2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="37">
         <v>45755</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="35"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="39"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
       <c r="G3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
       <c r="M3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="N3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="38"/>
-    </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="45"/>
+    </row>
+    <row r="4" spans="1:17" ht="30">
       <c r="A4" s="18" t="s">
         <v>9</v>
       </c>
@@ -1738,7 +1745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="45.75" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
@@ -1779,7 +1786,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="28.5">
       <c r="A6" s="16" t="s">
         <v>32</v>
       </c>
@@ -1824,7 +1831,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="28.5">
       <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1876,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="45.75" customHeight="1" thickBot="1">
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
@@ -1912,7 +1919,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="29.25" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>127</v>
       </c>
@@ -1955,7 +1962,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="43.5" thickBot="1">
       <c r="G10" s="17" t="s">
         <v>64</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="29.25" thickBot="1">
       <c r="G11" s="17" t="s">
         <v>65</v>
       </c>
@@ -2013,7 +2020,20 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="116.25" customHeight="1" thickBot="1">
+      <c r="G12" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>139</v>
+      </c>
       <c r="M12" s="16" t="s">
         <v>103</v>
       </c>
@@ -2028,76 +2048,76 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15">
       <c r="A13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="G13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="37">
         <v>45755</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="G14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="37">
         <v>45755</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1">
       <c r="A15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
       <c r="G15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
       <c r="M15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="32"/>
-    </row>
-    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="48"/>
+    </row>
+    <row r="16" spans="1:17" ht="30">
       <c r="A16" s="18" t="s">
         <v>9</v>
       </c>
@@ -2131,14 +2151,14 @@
       <c r="M16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="37">
         <v>45755</v>
       </c>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="35"/>
-    </row>
-    <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="39"/>
+    </row>
+    <row r="17" spans="1:17" ht="43.5" thickBot="1">
       <c r="A17" s="16" t="s">
         <v>43</v>
       </c>
@@ -2168,14 +2188,14 @@
       <c r="M17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N17" s="36" t="s">
+      <c r="N17" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="38"/>
-    </row>
-    <row r="18" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="45"/>
+    </row>
+    <row r="18" spans="1:17" ht="30">
       <c r="A18" s="16" t="s">
         <v>44</v>
       </c>
@@ -2222,7 +2242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="43.5" thickBot="1">
       <c r="A19" s="17" t="s">
         <v>45</v>
       </c>
@@ -2265,7 +2285,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="48" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>46</v>
       </c>
@@ -2310,7 +2330,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="44.25" customHeight="1" thickBot="1">
       <c r="A21" s="16" t="s">
         <v>47</v>
       </c>
@@ -2340,7 +2360,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="33" customHeight="1" thickBot="1">
       <c r="A22" s="17" t="s">
         <v>48</v>
       </c>
@@ -2357,12 +2377,12 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="32"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="48"/>
       <c r="M22" s="16" t="s">
         <v>121</v>
       </c>
@@ -2379,7 +2399,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="42.75" customHeight="1" thickBot="1">
       <c r="A23" s="17" t="s">
         <v>49</v>
       </c>
@@ -2398,12 +2418,12 @@
       <c r="G23" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="34">
         <v>45755</v>
       </c>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="48"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="36"/>
       <c r="M23" s="16" t="s">
         <v>122</v>
       </c>
@@ -2418,7 +2438,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="32.25" customHeight="1" thickBot="1">
       <c r="A24" s="17" t="s">
         <v>133</v>
       </c>
@@ -2432,18 +2452,18 @@
       <c r="E24" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="42"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="43" t="s">
+      <c r="H24" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="45"/>
-    </row>
-    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="33"/>
+    </row>
+    <row r="25" spans="1:17" ht="30">
       <c r="G25" s="18" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="42.75">
       <c r="G26" s="16" t="s">
         <v>85</v>
       </c>
@@ -2475,7 +2495,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="28.5">
       <c r="G27" s="16" t="s">
         <v>86</v>
       </c>
@@ -2492,7 +2512,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="28.5">
       <c r="G28" s="16" t="s">
         <v>87</v>
       </c>
@@ -2509,7 +2529,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="28.5">
       <c r="G29" s="16" t="s">
         <v>88</v>
       </c>
@@ -2528,6 +2548,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="H24:K24"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="B2:E2"/>
@@ -2538,16 +2568,6 @@
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>